<commit_message>
dataset ready for MSFT and GOOGL
</commit_message>
<xml_diff>
--- a/GOOGL/GOOGL - Cash Flow.xlsx
+++ b/GOOGL/GOOGL - Cash Flow.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1001566\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YiLong/Desktop/SUTD/Term 9 (SUTD)/50.038 - Computational Data Science/Project/cds/GOOGL/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4A74E3-CF3A-0C41-84DE-9FF4C97AAA56}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="-105" windowWidth="14850" windowHeight="12735"/>
+    <workbookView xWindow="10400" yWindow="460" windowWidth="14860" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Flow - As Reported" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="154">
   <si>
     <t>Alphabet Inc (GOOGL US) - As Reported</t>
   </si>
@@ -475,14 +476,20 @@
   </si>
   <si>
     <t>Source: Bloomberg</t>
+  </si>
+  <si>
+    <t>Q4 2014</t>
+  </si>
+  <si>
+    <t>12/31/2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1128,13 +1135,13 @@
     <xf numFmtId="3" fontId="1" fillId="34" borderId="2">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="34" borderId="2">
+    <xf numFmtId="164" fontId="1" fillId="34" borderId="2">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="34" borderId="2">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="34" borderId="2">
+    <xf numFmtId="164" fontId="7" fillId="34" borderId="2">
       <alignment horizontal="right"/>
     </xf>
   </cellStyleXfs>
@@ -1165,13 +1172,13 @@
     <xf numFmtId="3" fontId="1" fillId="34" borderId="2" xfId="52" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="34" borderId="2" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="34" borderId="2" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="34" borderId="2" xfId="54" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="34" borderId="2" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="34" borderId="2" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1201,23 +1208,23 @@
     <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="blp_column_header" xfId="26"/>
-    <cellStyle name="blp_title_header_row_left" xfId="50"/>
+    <cellStyle name="blp_column_header" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="blp_title_header_row_left" xfId="50" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Calculation" xfId="27" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="28" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="29" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="fa_column_header_bottom" xfId="30"/>
-    <cellStyle name="fa_column_header_bottom_left" xfId="51"/>
-    <cellStyle name="fa_column_header_empty" xfId="31"/>
-    <cellStyle name="fa_column_header_top" xfId="32"/>
-    <cellStyle name="fa_column_header_top_left" xfId="33"/>
-    <cellStyle name="fa_data_bold_0_grouped" xfId="54"/>
-    <cellStyle name="fa_data_bold_1_grouped" xfId="55"/>
-    <cellStyle name="fa_data_standard_0_grouped" xfId="52"/>
-    <cellStyle name="fa_data_standard_1_grouped" xfId="53"/>
-    <cellStyle name="fa_footer_italic" xfId="34"/>
-    <cellStyle name="fa_row_header_bold" xfId="35"/>
-    <cellStyle name="fa_row_header_standard" xfId="36"/>
+    <cellStyle name="fa_column_header_bottom" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="fa_column_header_bottom_left" xfId="51" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="fa_column_header_empty" xfId="31" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="fa_column_header_top" xfId="32" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="fa_column_header_top_left" xfId="33" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="fa_data_bold_0_grouped" xfId="54" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="fa_data_bold_1_grouped" xfId="55" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="fa_data_standard_0_grouped" xfId="52" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="fa_data_standard_1_grouped" xfId="53" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="fa_footer_italic" xfId="34" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="fa_row_header_bold" xfId="35" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="fa_row_header_standard" xfId="36" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Good" xfId="37" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="38" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="39" builtinId="17" customBuiltin="1"/>
@@ -1322,6 +1329,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1357,6 +1381,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1532,19 +1573,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP95"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AQ95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V40" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="42" width="11.85546875" customWidth="1"/>
+    <col min="3" max="43" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1587,8 +1630,9 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:42" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1633,8 +1677,9 @@
       <c r="AN2" s="8"/>
       <c r="AO2" s="8"/>
       <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1677,8 +1722,9 @@
       <c r="AN3" s="2"/>
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1759,52 +1805,55 @@
         <v>26</v>
       </c>
       <c r="AB4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AE4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AF4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AQ4" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>42</v>
       </c>
@@ -1885,52 +1934,55 @@
         <v>67</v>
       </c>
       <c r="AB5" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="AC5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AC5" s="5" t="s">
+      <c r="AD5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="AE5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AE5" s="5" t="s">
+      <c r="AF5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AF5" s="5" t="s">
+      <c r="AG5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="5" t="s">
+      <c r="AH5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AH5" s="5" t="s">
+      <c r="AI5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AI5" s="5" t="s">
+      <c r="AJ5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AJ5" s="5" t="s">
+      <c r="AK5" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AK5" s="5" t="s">
+      <c r="AL5" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AM5" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AN5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AO5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AP5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AP5" s="5" t="s">
+      <c r="AQ5" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>83</v>
       </c>
@@ -1975,8 +2027,9 @@
       <c r="AN6" s="13"/>
       <c r="AO6" s="13"/>
       <c r="AP6" s="13"/>
+      <c r="AQ6" s="13"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -2021,8 +2074,9 @@
       <c r="AN7" s="11"/>
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
+      <c r="AQ7" s="11"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
@@ -2102,53 +2156,54 @@
       <c r="AA8" s="12">
         <v>2739</v>
       </c>
-      <c r="AB8" s="12">
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12">
         <v>3515</v>
       </c>
-      <c r="AC8" s="12">
+      <c r="AD8" s="12">
         <v>3931</v>
       </c>
-      <c r="AD8" s="12">
+      <c r="AE8" s="12">
         <v>3979</v>
       </c>
-      <c r="AE8" s="12">
+      <c r="AF8" s="12">
         <v>4923</v>
       </c>
-      <c r="AF8" s="12">
+      <c r="AG8" s="12">
         <v>4207</v>
       </c>
-      <c r="AG8" s="12">
+      <c r="AH8" s="12">
         <v>4877</v>
       </c>
-      <c r="AH8" s="12">
+      <c r="AI8" s="12">
         <v>5061</v>
       </c>
-      <c r="AI8" s="12">
+      <c r="AJ8" s="12">
         <v>5333</v>
       </c>
-      <c r="AJ8" s="12">
+      <c r="AK8" s="12">
         <v>5426</v>
       </c>
-      <c r="AK8" s="12">
+      <c r="AL8" s="12">
         <v>3524</v>
       </c>
-      <c r="AL8" s="12">
+      <c r="AM8" s="12">
         <v>6732</v>
       </c>
-      <c r="AM8" s="12">
+      <c r="AN8" s="12">
         <v>-3020</v>
       </c>
-      <c r="AN8" s="12">
+      <c r="AO8" s="12">
         <v>9401</v>
       </c>
-      <c r="AO8" s="12">
+      <c r="AP8" s="12">
         <v>3195</v>
       </c>
-      <c r="AP8" s="12">
+      <c r="AQ8" s="12">
         <v>9192</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
@@ -2228,53 +2283,54 @@
       <c r="AA9" s="12">
         <v>884</v>
       </c>
-      <c r="AB9" s="12">
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12">
         <v>938</v>
       </c>
-      <c r="AC9" s="12">
+      <c r="AD9" s="12">
         <v>1011</v>
       </c>
-      <c r="AD9" s="12">
+      <c r="AE9" s="12">
         <v>1030</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AF9" s="12">
         <v>1153</v>
       </c>
-      <c r="AF9" s="12">
+      <c r="AG9" s="12">
         <v>1155</v>
       </c>
-      <c r="AG9" s="12">
+      <c r="AH9" s="12">
         <v>1271</v>
       </c>
-      <c r="AH9" s="12">
+      <c r="AI9" s="12">
         <v>1377</v>
       </c>
-      <c r="AI9" s="12">
+      <c r="AJ9" s="12">
         <v>1464</v>
       </c>
-      <c r="AJ9" s="12">
+      <c r="AK9" s="12">
         <v>1287</v>
       </c>
-      <c r="AK9" s="12">
+      <c r="AL9" s="12">
         <v>1424</v>
       </c>
-      <c r="AL9" s="12">
+      <c r="AM9" s="12">
         <v>1561</v>
       </c>
-      <c r="AM9" s="12">
+      <c r="AN9" s="12">
         <v>1831</v>
       </c>
-      <c r="AN9" s="12">
+      <c r="AO9" s="12">
         <v>1791</v>
       </c>
-      <c r="AO9" s="12">
+      <c r="AP9" s="12">
         <v>1862</v>
       </c>
-      <c r="AP9" s="12">
+      <c r="AQ9" s="12">
         <v>2138</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>88</v>
       </c>
@@ -2354,9 +2410,7 @@
       <c r="AA10" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB10" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB10" s="12"/>
       <c r="AC10" s="12" t="s">
         <v>87</v>
       </c>
@@ -2399,8 +2453,11 @@
       <c r="AP10" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ10" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
@@ -2480,53 +2537,54 @@
       <c r="AA11" s="12">
         <v>-360</v>
       </c>
-      <c r="AB11" s="12">
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12">
         <v>71</v>
       </c>
-      <c r="AC11" s="12">
+      <c r="AD11" s="12">
         <v>-221</v>
       </c>
-      <c r="AD11" s="12">
+      <c r="AE11" s="12">
         <v>-416</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AF11" s="12">
         <v>387</v>
       </c>
-      <c r="AF11" s="12">
+      <c r="AG11" s="12">
         <v>414</v>
       </c>
-      <c r="AG11" s="12">
+      <c r="AH11" s="12">
         <v>-50</v>
       </c>
-      <c r="AH11" s="12">
+      <c r="AI11" s="12">
         <v>-245</v>
       </c>
-      <c r="AI11" s="12">
+      <c r="AJ11" s="12">
         <v>-157</v>
       </c>
-      <c r="AJ11" s="12">
+      <c r="AK11" s="12">
         <v>613</v>
       </c>
-      <c r="AK11" s="12">
+      <c r="AL11" s="12">
         <v>-75</v>
       </c>
-      <c r="AL11" s="12">
+      <c r="AM11" s="12">
         <v>-296</v>
       </c>
-      <c r="AM11" s="12">
+      <c r="AN11" s="12">
         <v>16</v>
       </c>
-      <c r="AN11" s="12">
+      <c r="AO11" s="12">
         <v>-18</v>
       </c>
-      <c r="AO11" s="12">
+      <c r="AP11" s="12">
         <v>-139</v>
       </c>
-      <c r="AP11" s="12">
+      <c r="AQ11" s="12">
         <v>880</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>90</v>
       </c>
@@ -2606,9 +2664,7 @@
       <c r="AA12" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB12" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB12" s="12"/>
       <c r="AC12" s="12" t="s">
         <v>87</v>
       </c>
@@ -2651,8 +2707,11 @@
       <c r="AP12" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ12" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>90</v>
       </c>
@@ -2732,9 +2791,7 @@
       <c r="AA13" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB13" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB13" s="12"/>
       <c r="AC13" s="12" t="s">
         <v>87</v>
       </c>
@@ -2777,8 +2834,11 @@
       <c r="AP13" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ13" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>91</v>
       </c>
@@ -2858,24 +2918,22 @@
       <c r="AA14" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB14" s="12">
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12">
         <v>1203</v>
       </c>
-      <c r="AC14" s="12">
+      <c r="AD14" s="12">
         <v>1132</v>
       </c>
-      <c r="AD14" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE14" s="12">
+      <c r="AE14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF14" s="12">
         <v>1436</v>
       </c>
-      <c r="AF14" s="12">
+      <c r="AG14" s="12">
         <v>1494</v>
       </c>
-      <c r="AG14" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AH14" s="12" t="s">
         <v>87</v>
       </c>
@@ -2885,26 +2943,29 @@
       <c r="AJ14" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AK14" s="12">
+      <c r="AK14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL14" s="12">
         <v>2003</v>
       </c>
-      <c r="AL14" s="12">
+      <c r="AM14" s="12">
         <v>1820</v>
       </c>
-      <c r="AM14" s="12">
+      <c r="AN14" s="12">
         <v>1847</v>
       </c>
-      <c r="AN14" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO14" s="12">
+      <c r="AO14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP14" s="12">
         <v>2413</v>
       </c>
-      <c r="AP14" s="12">
+      <c r="AQ14" s="12">
         <v>2230</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>91</v>
       </c>
@@ -2984,53 +3045,54 @@
       <c r="AA15" s="12">
         <v>1290</v>
       </c>
-      <c r="AB15" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB15" s="12"/>
       <c r="AC15" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD15" s="12">
+      <c r="AD15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE15" s="12">
         <v>1432</v>
       </c>
-      <c r="AE15" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AF15" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG15" s="12">
+      <c r="AG15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH15" s="12">
         <v>1503</v>
       </c>
-      <c r="AH15" s="12">
+      <c r="AI15" s="12">
         <v>1860</v>
       </c>
-      <c r="AI15" s="12">
+      <c r="AJ15" s="12">
         <v>1846</v>
       </c>
-      <c r="AJ15" s="12">
+      <c r="AK15" s="12">
         <v>2009</v>
       </c>
-      <c r="AK15" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AL15" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AM15" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AN15" s="12">
+      <c r="AN15" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO15" s="12">
         <v>2457</v>
       </c>
-      <c r="AO15" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AP15" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ15" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>92</v>
       </c>
@@ -3110,53 +3172,54 @@
       <c r="AA16" s="12">
         <v>66</v>
       </c>
-      <c r="AB16" s="12">
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12">
         <v>61</v>
       </c>
-      <c r="AC16" s="12">
+      <c r="AD16" s="12">
         <v>55</v>
       </c>
-      <c r="AD16" s="12">
+      <c r="AE16" s="12">
         <v>41</v>
       </c>
-      <c r="AE16" s="12">
+      <c r="AF16" s="12">
         <v>55</v>
       </c>
-      <c r="AF16" s="12">
+      <c r="AG16" s="12">
         <v>64</v>
       </c>
-      <c r="AG16" s="12">
+      <c r="AH16" s="12">
         <v>27</v>
       </c>
-      <c r="AH16" s="12">
+      <c r="AI16" s="12">
         <v>26</v>
-      </c>
-      <c r="AI16" s="12">
-        <v>57</v>
       </c>
       <c r="AJ16" s="12">
         <v>57</v>
       </c>
       <c r="AK16" s="12">
+        <v>57</v>
+      </c>
+      <c r="AL16" s="12">
         <v>39</v>
       </c>
-      <c r="AL16" s="12">
+      <c r="AM16" s="12">
         <v>96</v>
       </c>
-      <c r="AM16" s="12">
+      <c r="AN16" s="12">
         <v>38</v>
       </c>
-      <c r="AN16" s="12">
+      <c r="AO16" s="12">
         <v>-257</v>
       </c>
-      <c r="AO16" s="12">
+      <c r="AP16" s="12">
         <v>137</v>
       </c>
-      <c r="AP16" s="12">
+      <c r="AQ16" s="12">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>93</v>
       </c>
@@ -3236,9 +3299,7 @@
       <c r="AA17" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB17" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB17" s="12"/>
       <c r="AC17" s="12" t="s">
         <v>87</v>
       </c>
@@ -3281,8 +3342,11 @@
       <c r="AP17" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ17" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>93</v>
       </c>
@@ -3362,9 +3426,7 @@
       <c r="AA18" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB18" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB18" s="12"/>
       <c r="AC18" s="12" t="s">
         <v>87</v>
       </c>
@@ -3407,8 +3469,11 @@
       <c r="AP18" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ18" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>94</v>
       </c>
@@ -3488,12 +3553,10 @@
       <c r="AA19" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB19" s="12">
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12">
         <v>-24</v>
       </c>
-      <c r="AC19" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AD19" s="12" t="s">
         <v>87</v>
       </c>
@@ -3503,12 +3566,12 @@
       <c r="AF19" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG19" s="12">
+      <c r="AG19" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH19" s="12">
         <v>48</v>
       </c>
-      <c r="AH19" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI19" s="12" t="s">
         <v>87</v>
       </c>
@@ -3533,8 +3596,11 @@
       <c r="AP19" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ19" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>94</v>
       </c>
@@ -3614,53 +3680,54 @@
       <c r="AA20" s="12">
         <v>-127</v>
       </c>
-      <c r="AB20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC20" s="12">
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD20" s="12">
         <v>-374</v>
       </c>
-      <c r="AD20" s="12">
+      <c r="AE20" s="12">
         <v>230</v>
       </c>
-      <c r="AE20" s="12">
+      <c r="AF20" s="12">
         <v>371</v>
       </c>
-      <c r="AF20" s="12">
+      <c r="AG20" s="12">
         <v>-269</v>
       </c>
-      <c r="AG20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH20" s="12">
+      <c r="AH20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI20" s="12">
         <v>459</v>
       </c>
-      <c r="AI20" s="12">
+      <c r="AJ20" s="12">
         <v>-128</v>
       </c>
-      <c r="AJ20" s="12">
+      <c r="AK20" s="12">
         <v>103</v>
       </c>
-      <c r="AK20" s="12">
+      <c r="AL20" s="12">
         <v>16</v>
       </c>
-      <c r="AL20" s="12">
+      <c r="AM20" s="12">
         <v>-61</v>
       </c>
-      <c r="AM20" s="12">
+      <c r="AN20" s="12">
         <v>673</v>
       </c>
-      <c r="AN20" s="12">
+      <c r="AO20" s="12">
         <v>122</v>
       </c>
-      <c r="AO20" s="12">
+      <c r="AP20" s="12">
         <v>-145</v>
       </c>
-      <c r="AP20" s="12">
+      <c r="AQ20" s="12">
         <v>316</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>95</v>
       </c>
@@ -3740,53 +3807,54 @@
       <c r="AA21" s="12">
         <v>-36</v>
       </c>
-      <c r="AB21" s="12">
+      <c r="AB21" s="12"/>
+      <c r="AC21" s="12">
         <v>698</v>
       </c>
-      <c r="AC21" s="12">
+      <c r="AD21" s="12">
         <v>-767</v>
       </c>
-      <c r="AD21" s="12">
+      <c r="AE21" s="12">
         <v>-267</v>
       </c>
-      <c r="AE21" s="12">
+      <c r="AF21" s="12">
         <v>-1758</v>
       </c>
-      <c r="AF21" s="12">
+      <c r="AG21" s="12">
         <v>818</v>
       </c>
-      <c r="AG21" s="12">
+      <c r="AH21" s="12">
         <v>-835</v>
       </c>
-      <c r="AH21" s="12">
+      <c r="AI21" s="12">
         <v>-282</v>
       </c>
-      <c r="AI21" s="12">
+      <c r="AJ21" s="12">
         <v>-2279</v>
       </c>
-      <c r="AJ21" s="12">
+      <c r="AK21" s="12">
         <v>1267</v>
       </c>
-      <c r="AK21" s="12">
+      <c r="AL21" s="12">
         <v>-836</v>
       </c>
-      <c r="AL21" s="12">
+      <c r="AM21" s="12">
         <v>-1150</v>
       </c>
-      <c r="AM21" s="12">
+      <c r="AN21" s="12">
         <v>-3049</v>
       </c>
-      <c r="AN21" s="12">
+      <c r="AO21" s="12">
         <v>1700</v>
       </c>
-      <c r="AO21" s="12">
+      <c r="AP21" s="12">
         <v>-312</v>
       </c>
-      <c r="AP21" s="12">
+      <c r="AQ21" s="12">
         <v>-670</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>96</v>
       </c>
@@ -3866,53 +3934,54 @@
       <c r="AA22" s="12">
         <v>-13</v>
       </c>
-      <c r="AB22" s="12">
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12">
         <v>43</v>
       </c>
-      <c r="AC22" s="12">
+      <c r="AD22" s="12">
         <v>19</v>
       </c>
-      <c r="AD22" s="12">
+      <c r="AE22" s="12">
         <v>142</v>
       </c>
-      <c r="AE22" s="12">
+      <c r="AF22" s="12">
         <v>-522</v>
       </c>
-      <c r="AF22" s="12">
+      <c r="AG22" s="12">
         <v>185</v>
       </c>
-      <c r="AG22" s="12">
+      <c r="AH22" s="12">
         <v>-24</v>
       </c>
-      <c r="AH22" s="12">
+      <c r="AI22" s="12">
         <v>-47</v>
       </c>
-      <c r="AI22" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AJ22" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AK22" s="12">
+      <c r="AK22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL22" s="12">
         <v>-326</v>
       </c>
-      <c r="AL22" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM22" s="12">
+      <c r="AM22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN22" s="12">
         <v>-78</v>
       </c>
-      <c r="AN22" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO22" s="12">
+      <c r="AO22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP22" s="12">
         <v>-515</v>
       </c>
-      <c r="AP22" s="12" t="s">
+      <c r="AQ22" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>97</v>
       </c>
@@ -3992,53 +4061,54 @@
       <c r="AA23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB23" s="12">
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12">
         <v>-205</v>
       </c>
-      <c r="AC23" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AD23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AE23" s="12">
+      <c r="AE23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF23" s="12">
         <v>777</v>
       </c>
-      <c r="AF23" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG23" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AH23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI23" s="12">
+      <c r="AI23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ23" s="12">
         <v>455</v>
       </c>
-      <c r="AJ23" s="12">
+      <c r="AK23" s="12">
         <v>-1868</v>
       </c>
-      <c r="AK23" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AL23" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AM23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AN23" s="12">
+      <c r="AN23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO23" s="12">
         <v>-1142</v>
       </c>
-      <c r="AO23" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AP23" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ23" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>97</v>
       </c>
@@ -4118,12 +4188,10 @@
       <c r="AA24" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB24" s="12">
+      <c r="AB24" s="12"/>
+      <c r="AC24" s="12">
         <v>-601</v>
       </c>
-      <c r="AC24" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AD24" s="12" t="s">
         <v>87</v>
       </c>
@@ -4163,8 +4231,11 @@
       <c r="AP24" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ24" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>97</v>
       </c>
@@ -4244,53 +4315,54 @@
       <c r="AA25" s="12">
         <v>484</v>
       </c>
-      <c r="AB25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC25" s="12">
+      <c r="AB25" s="12"/>
+      <c r="AC25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD25" s="12">
         <v>84</v>
       </c>
-      <c r="AD25" s="12">
+      <c r="AE25" s="12">
         <v>583</v>
       </c>
-      <c r="AE25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF25" s="12">
+      <c r="AF25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG25" s="12">
         <v>-1064</v>
       </c>
-      <c r="AG25" s="12">
+      <c r="AH25" s="12">
         <v>593</v>
       </c>
-      <c r="AH25" s="12">
+      <c r="AI25" s="12">
         <v>809</v>
       </c>
-      <c r="AI25" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AJ25" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AK25" s="12">
+      <c r="AK25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL25" s="12">
         <v>3555</v>
       </c>
-      <c r="AL25" s="12">
+      <c r="AM25" s="12">
         <v>1434</v>
       </c>
-      <c r="AM25" s="12">
+      <c r="AN25" s="12">
         <v>1770</v>
       </c>
-      <c r="AN25" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO25" s="12">
+      <c r="AO25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP25" s="12">
         <v>5742</v>
       </c>
-      <c r="AP25" s="12">
+      <c r="AQ25" s="12">
         <v>1857</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>98</v>
       </c>
@@ -4370,53 +4442,54 @@
       <c r="AA26" s="12">
         <v>104</v>
       </c>
-      <c r="AB26" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC26" s="12">
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD26" s="12">
         <v>838</v>
       </c>
-      <c r="AD26" s="12">
+      <c r="AE26" s="12">
         <v>52</v>
       </c>
-      <c r="AE26" s="12">
+      <c r="AF26" s="12">
         <v>408</v>
       </c>
-      <c r="AF26" s="12">
+      <c r="AG26" s="12">
         <v>-131</v>
       </c>
-      <c r="AG26" s="12">
+      <c r="AH26" s="12">
         <v>83</v>
       </c>
-      <c r="AH26" s="12">
+      <c r="AI26" s="12">
         <v>186</v>
       </c>
-      <c r="AI26" s="12">
+      <c r="AJ26" s="12">
         <v>1177</v>
       </c>
-      <c r="AJ26" s="12">
+      <c r="AK26" s="12">
         <v>-74</v>
       </c>
-      <c r="AK26" s="12">
+      <c r="AL26" s="12">
         <v>80</v>
       </c>
-      <c r="AL26" s="12">
+      <c r="AM26" s="12">
         <v>176</v>
       </c>
-      <c r="AM26" s="12">
+      <c r="AN26" s="12">
         <v>773</v>
       </c>
-      <c r="AN26" s="12">
+      <c r="AO26" s="12">
         <v>-286</v>
       </c>
-      <c r="AO26" s="12">
+      <c r="AP26" s="12">
         <v>-17</v>
       </c>
-      <c r="AP26" s="12">
+      <c r="AQ26" s="12">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>99</v>
       </c>
@@ -4496,12 +4569,10 @@
       <c r="AA27" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB27" s="12">
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12">
         <v>-59</v>
       </c>
-      <c r="AC27" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AD27" s="12" t="s">
         <v>87</v>
       </c>
@@ -4541,8 +4612,11 @@
       <c r="AP27" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ27" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>99</v>
       </c>
@@ -4622,53 +4696,54 @@
       <c r="AA28" s="12">
         <v>0</v>
       </c>
-      <c r="AB28" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC28" s="12">
+      <c r="AB28" s="12"/>
+      <c r="AC28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD28" s="12">
         <v>25</v>
       </c>
-      <c r="AD28" s="12">
+      <c r="AE28" s="12">
         <v>-21</v>
       </c>
-      <c r="AE28" s="12">
+      <c r="AF28" s="12">
         <v>98</v>
       </c>
-      <c r="AF28" s="12">
+      <c r="AG28" s="12">
         <v>18</v>
       </c>
-      <c r="AG28" s="12">
+      <c r="AH28" s="12">
         <v>-15</v>
       </c>
-      <c r="AH28" s="12">
+      <c r="AI28" s="12">
         <v>39</v>
       </c>
-      <c r="AI28" s="12">
+      <c r="AJ28" s="12">
         <v>181</v>
       </c>
-      <c r="AJ28" s="12">
+      <c r="AK28" s="12">
         <v>111</v>
       </c>
-      <c r="AK28" s="12">
+      <c r="AL28" s="12">
         <v>84</v>
       </c>
-      <c r="AL28" s="12">
+      <c r="AM28" s="12">
         <v>33</v>
       </c>
-      <c r="AM28" s="12">
+      <c r="AN28" s="12">
         <v>162</v>
       </c>
-      <c r="AN28" s="12">
+      <c r="AO28" s="12">
         <v>130</v>
       </c>
-      <c r="AO28" s="12">
+      <c r="AP28" s="12">
         <v>165</v>
       </c>
-      <c r="AP28" s="12">
+      <c r="AQ28" s="12">
         <v>-23</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>100</v>
       </c>
@@ -4748,53 +4823,54 @@
       <c r="AA29" s="12">
         <v>487</v>
       </c>
-      <c r="AB29" s="12">
+      <c r="AB29" s="12"/>
+      <c r="AC29" s="12">
         <v>827</v>
       </c>
-      <c r="AC29" s="12">
+      <c r="AD29" s="12">
         <v>1123</v>
       </c>
-      <c r="AD29" s="12">
+      <c r="AE29" s="12">
         <v>-857</v>
       </c>
-      <c r="AE29" s="12">
+      <c r="AF29" s="12">
         <v>-1272</v>
       </c>
-      <c r="AF29" s="12">
+      <c r="AG29" s="12">
         <v>271</v>
       </c>
-      <c r="AG29" s="12">
+      <c r="AH29" s="12">
         <v>1409</v>
       </c>
-      <c r="AH29" s="12">
+      <c r="AI29" s="12">
         <v>473</v>
       </c>
-      <c r="AI29" s="12">
+      <c r="AJ29" s="12">
         <v>972</v>
       </c>
-      <c r="AJ29" s="12">
+      <c r="AK29" s="12">
         <v>510</v>
       </c>
-      <c r="AK29" s="12">
+      <c r="AL29" s="12">
         <v>-2289</v>
       </c>
-      <c r="AL29" s="12">
+      <c r="AM29" s="12">
         <v>914</v>
       </c>
-      <c r="AM29" s="12">
+      <c r="AN29" s="12">
         <v>9076</v>
       </c>
-      <c r="AN29" s="12">
+      <c r="AO29" s="12">
         <v>782</v>
       </c>
-      <c r="AO29" s="12">
+      <c r="AP29" s="12">
         <v>-1438</v>
       </c>
-      <c r="AP29" s="12">
+      <c r="AQ29" s="12">
         <v>-1235</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
         <v>101</v>
       </c>
@@ -4874,9 +4950,7 @@
       <c r="AA30" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB30" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB30" s="12"/>
       <c r="AC30" s="12" t="s">
         <v>87</v>
       </c>
@@ -4919,8 +4993,11 @@
       <c r="AP30" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ30" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>102</v>
       </c>
@@ -5000,9 +5077,7 @@
       <c r="AA31" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB31" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB31" s="12"/>
       <c r="AC31" s="12" t="s">
         <v>87</v>
       </c>
@@ -5045,8 +5120,11 @@
       <c r="AP31" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ31" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
         <v>103</v>
       </c>
@@ -5126,9 +5204,7 @@
       <c r="AA32" s="12">
         <v>-175</v>
       </c>
-      <c r="AB32" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB32" s="12"/>
       <c r="AC32" s="12" t="s">
         <v>87</v>
       </c>
@@ -5171,8 +5247,11 @@
       <c r="AP32" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ32" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>104</v>
       </c>
@@ -5252,53 +5331,54 @@
       <c r="AA33" s="12">
         <v>663</v>
       </c>
-      <c r="AB33" s="12">
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12">
         <v>239</v>
       </c>
-      <c r="AC33" s="12">
+      <c r="AD33" s="12">
         <v>223</v>
       </c>
-      <c r="AD33" s="12">
+      <c r="AE33" s="12">
         <v>218</v>
       </c>
-      <c r="AE33" s="12">
+      <c r="AF33" s="12">
         <v>251</v>
       </c>
-      <c r="AF33" s="12">
+      <c r="AG33" s="12">
         <v>216</v>
-      </c>
-      <c r="AG33" s="12">
-        <v>219</v>
       </c>
       <c r="AH33" s="12">
         <v>219</v>
       </c>
       <c r="AI33" s="12">
+        <v>219</v>
+      </c>
+      <c r="AJ33" s="12">
         <v>223</v>
       </c>
-      <c r="AJ33" s="12">
+      <c r="AK33" s="12">
         <v>216</v>
       </c>
-      <c r="AK33" s="12">
+      <c r="AL33" s="12">
         <v>201</v>
       </c>
-      <c r="AL33" s="12">
+      <c r="AM33" s="12">
         <v>200</v>
-      </c>
-      <c r="AM33" s="12">
-        <v>195</v>
       </c>
       <c r="AN33" s="12">
         <v>195</v>
       </c>
       <c r="AO33" s="12">
+        <v>195</v>
+      </c>
+      <c r="AP33" s="12">
         <v>252</v>
       </c>
-      <c r="AP33" s="12">
+      <c r="AQ33" s="12">
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>105</v>
       </c>
@@ -5378,9 +5458,7 @@
       <c r="AA34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB34" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB34" s="12"/>
       <c r="AC34" s="12" t="s">
         <v>87</v>
       </c>
@@ -5399,32 +5477,35 @@
       <c r="AH34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI34" s="12">
+      <c r="AI34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ34" s="12">
         <v>198</v>
       </c>
-      <c r="AJ34" s="12">
+      <c r="AK34" s="12">
         <v>-128</v>
       </c>
-      <c r="AK34" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AL34" s="12">
+      <c r="AL34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM34" s="12">
         <v>-1632</v>
       </c>
-      <c r="AM34" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN34" s="12">
+      <c r="AN34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO34" s="12">
         <v>-241</v>
       </c>
-      <c r="AO34" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AP34" s="12">
+      <c r="AP34" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ34" s="12">
         <v>-484</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
         <v>106</v>
       </c>
@@ -5504,53 +5585,54 @@
       <c r="AA35" s="12">
         <v>5994</v>
       </c>
-      <c r="AB35" s="12">
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12">
         <v>6722</v>
       </c>
-      <c r="AC35" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD35" s="12">
+      <c r="AD35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE35" s="12">
         <v>6145</v>
       </c>
-      <c r="AE35" s="12">
+      <c r="AF35" s="12">
         <v>6609</v>
       </c>
-      <c r="AF35" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG35" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AH35" s="12">
+      <c r="AH35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI35" s="12">
         <v>9845</v>
       </c>
-      <c r="AI35" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AJ35" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AK35" s="12">
+      <c r="AK35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL35" s="12">
         <v>7403</v>
       </c>
-      <c r="AL35" s="12">
+      <c r="AM35" s="12">
         <v>9872</v>
       </c>
-      <c r="AM35" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AN35" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AO35" s="12">
+      <c r="AO35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP35" s="12">
         <v>10132</v>
       </c>
-      <c r="AP35" s="12">
+      <c r="AQ35" s="12">
         <v>13210</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>106</v>
       </c>
@@ -5630,53 +5712,54 @@
       <c r="AA36" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB36" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC36" s="12">
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD36" s="12">
         <v>7096</v>
       </c>
-      <c r="AD36" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AE36" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AF36" s="12">
+      <c r="AF36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG36" s="12">
         <v>7658</v>
       </c>
-      <c r="AG36" s="12">
+      <c r="AH36" s="12">
         <v>9120</v>
       </c>
-      <c r="AH36" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI36" s="12">
+      <c r="AI36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ36" s="12">
         <v>9413</v>
       </c>
-      <c r="AJ36" s="12">
+      <c r="AK36" s="12">
         <v>9548</v>
       </c>
-      <c r="AK36" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AL36" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AM36" s="12">
+      <c r="AM36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN36" s="12">
         <v>10268</v>
       </c>
-      <c r="AN36" s="12">
+      <c r="AO36" s="12">
         <v>11642</v>
       </c>
-      <c r="AO36" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AP36" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ36" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>107</v>
       </c>
@@ -5756,53 +5839,54 @@
       <c r="AA37" s="12">
         <v>-12</v>
       </c>
-      <c r="AB37" s="12">
+      <c r="AB37" s="12"/>
+      <c r="AC37" s="12">
         <v>16</v>
       </c>
-      <c r="AC37" s="12">
+      <c r="AD37" s="12">
         <v>17</v>
       </c>
-      <c r="AD37" s="12">
+      <c r="AE37" s="12">
         <v>-1</v>
       </c>
-      <c r="AE37" s="12">
+      <c r="AF37" s="12">
         <v>302</v>
       </c>
-      <c r="AF37" s="12">
+      <c r="AG37" s="12">
         <v>280</v>
       </c>
-      <c r="AG37" s="12">
+      <c r="AH37" s="12">
         <v>14</v>
       </c>
-      <c r="AH37" s="12">
+      <c r="AI37" s="12">
         <v>-90</v>
       </c>
-      <c r="AI37" s="12">
+      <c r="AJ37" s="12">
         <v>71</v>
       </c>
-      <c r="AJ37" s="12">
+      <c r="AK37" s="12">
         <v>19</v>
       </c>
-      <c r="AK37" s="12">
+      <c r="AL37" s="12">
         <v>3</v>
       </c>
-      <c r="AL37" s="12">
+      <c r="AM37" s="12">
         <v>45</v>
       </c>
-      <c r="AM37" s="12">
+      <c r="AN37" s="12">
         <v>34</v>
       </c>
-      <c r="AN37" s="12">
+      <c r="AO37" s="12">
         <v>-2992</v>
       </c>
-      <c r="AO37" s="12">
+      <c r="AP37" s="12">
         <v>-1068</v>
       </c>
-      <c r="AP37" s="12">
+      <c r="AQ37" s="12">
         <v>-1353</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
         <v>108</v>
       </c>
@@ -5882,9 +5966,7 @@
       <c r="AA38" s="12">
         <v>0</v>
       </c>
-      <c r="AB38" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB38" s="12"/>
       <c r="AC38" s="12" t="s">
         <v>87</v>
       </c>
@@ -5927,8 +6009,11 @@
       <c r="AP38" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ38" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
         <v>109</v>
       </c>
@@ -5973,8 +6058,9 @@
       <c r="AN39" s="11"/>
       <c r="AO39" s="11"/>
       <c r="AP39" s="11"/>
+      <c r="AQ39" s="11"/>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>110</v>
       </c>
@@ -6054,53 +6140,54 @@
       <c r="AA40" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB40" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB40" s="12"/>
       <c r="AC40" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD40" s="12">
+      <c r="AD40" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE40" s="12">
         <v>10</v>
       </c>
-      <c r="AE40" s="12">
+      <c r="AF40" s="12">
         <v>2</v>
       </c>
-      <c r="AF40" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG40" s="12">
+      <c r="AG40" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH40" s="12">
         <v>13</v>
       </c>
-      <c r="AH40" s="12">
+      <c r="AI40" s="12">
         <v>197</v>
       </c>
-      <c r="AI40" s="12">
+      <c r="AJ40" s="12">
         <v>14</v>
       </c>
-      <c r="AJ40" s="12">
+      <c r="AK40" s="12">
         <v>41</v>
       </c>
-      <c r="AK40" s="12">
+      <c r="AL40" s="12">
         <v>13</v>
       </c>
-      <c r="AL40" s="12">
+      <c r="AM40" s="12">
         <v>27</v>
       </c>
-      <c r="AM40" s="12">
+      <c r="AN40" s="12">
         <v>18</v>
       </c>
-      <c r="AN40" s="12">
+      <c r="AO40" s="12">
         <v>30</v>
       </c>
-      <c r="AO40" s="12">
+      <c r="AP40" s="12">
         <v>19</v>
       </c>
-      <c r="AP40" s="12">
+      <c r="AQ40" s="12">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>111</v>
       </c>
@@ -6180,53 +6267,54 @@
       <c r="AA41" s="12">
         <v>-2417</v>
       </c>
-      <c r="AB41" s="12">
+      <c r="AB41" s="12"/>
+      <c r="AC41" s="12">
         <v>-2927</v>
       </c>
-      <c r="AC41" s="12">
+      <c r="AD41" s="12">
         <v>-2515</v>
       </c>
-      <c r="AD41" s="12">
+      <c r="AE41" s="12">
         <v>-2383</v>
       </c>
-      <c r="AE41" s="12">
+      <c r="AF41" s="12">
         <v>-2102</v>
       </c>
-      <c r="AF41" s="12">
+      <c r="AG41" s="12">
         <v>-2428</v>
       </c>
-      <c r="AG41" s="12">
+      <c r="AH41" s="12">
         <v>-2136</v>
       </c>
-      <c r="AH41" s="12">
+      <c r="AI41" s="12">
         <v>-2554</v>
       </c>
-      <c r="AI41" s="12">
+      <c r="AJ41" s="12">
         <v>-3078</v>
       </c>
-      <c r="AJ41" s="12">
+      <c r="AK41" s="12">
         <v>-2508</v>
       </c>
-      <c r="AK41" s="12">
+      <c r="AL41" s="12">
         <v>-2831</v>
       </c>
-      <c r="AL41" s="12">
+      <c r="AM41" s="12">
         <v>-3538</v>
       </c>
-      <c r="AM41" s="12">
+      <c r="AN41" s="12">
         <v>-4307</v>
       </c>
-      <c r="AN41" s="12">
+      <c r="AO41" s="12">
         <v>-7299</v>
       </c>
-      <c r="AO41" s="12">
+      <c r="AP41" s="12">
         <v>-5477</v>
       </c>
-      <c r="AP41" s="12">
+      <c r="AQ41" s="12">
         <v>-5282</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>112</v>
       </c>
@@ -6306,9 +6394,7 @@
       <c r="AA42" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB42" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB42" s="12"/>
       <c r="AC42" s="12" t="s">
         <v>87</v>
       </c>
@@ -6321,18 +6407,18 @@
       <c r="AF42" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG42" s="12">
+      <c r="AG42" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH42" s="12">
         <v>56</v>
       </c>
-      <c r="AH42" s="12">
+      <c r="AI42" s="12">
         <v>91</v>
       </c>
-      <c r="AI42" s="12">
+      <c r="AJ42" s="12">
         <v>305</v>
       </c>
-      <c r="AJ42" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK42" s="12" t="s">
         <v>87</v>
       </c>
@@ -6351,8 +6437,11 @@
       <c r="AP42" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ42" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>113</v>
       </c>
@@ -6432,53 +6521,54 @@
       <c r="AA43" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB43" s="12">
+      <c r="AB43" s="12"/>
+      <c r="AC43" s="12">
         <v>-1074</v>
       </c>
-      <c r="AC43" s="12">
+      <c r="AD43" s="12">
         <v>-375</v>
       </c>
-      <c r="AD43" s="12">
+      <c r="AE43" s="12">
         <v>-322</v>
       </c>
-      <c r="AE43" s="12">
+      <c r="AF43" s="12">
         <v>-406</v>
       </c>
-      <c r="AF43" s="12">
+      <c r="AG43" s="12">
         <v>-321</v>
       </c>
-      <c r="AG43" s="12">
+      <c r="AH43" s="12">
         <v>-318</v>
       </c>
-      <c r="AH43" s="12">
+      <c r="AI43" s="12">
         <v>-181</v>
       </c>
-      <c r="AI43" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ43" s="12">
+      <c r="AJ43" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK43" s="12">
         <v>-354</v>
       </c>
-      <c r="AK43" s="12">
+      <c r="AL43" s="12">
         <v>-340</v>
       </c>
-      <c r="AL43" s="12">
+      <c r="AM43" s="12">
         <v>-177</v>
       </c>
-      <c r="AM43" s="12">
+      <c r="AN43" s="12">
         <v>-874</v>
       </c>
-      <c r="AN43" s="12">
+      <c r="AO43" s="12">
         <v>-327</v>
       </c>
-      <c r="AO43" s="12">
+      <c r="AP43" s="12">
         <v>-405</v>
       </c>
-      <c r="AP43" s="12">
+      <c r="AQ43" s="12">
         <v>-386</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>113</v>
       </c>
@@ -6558,9 +6648,7 @@
       <c r="AA44" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB44" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB44" s="12"/>
       <c r="AC44" s="12" t="s">
         <v>87</v>
       </c>
@@ -6579,12 +6667,12 @@
       <c r="AH44" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI44" s="12">
+      <c r="AI44" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ44" s="12">
         <v>-247</v>
       </c>
-      <c r="AJ44" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK44" s="12" t="s">
         <v>87</v>
       </c>
@@ -6603,8 +6691,11 @@
       <c r="AP44" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ44" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>114</v>
       </c>
@@ -6684,9 +6775,7 @@
       <c r="AA45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB45" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB45" s="12"/>
       <c r="AC45" s="12" t="s">
         <v>87</v>
       </c>
@@ -6708,29 +6797,32 @@
       <c r="AI45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AJ45" s="12">
+      <c r="AJ45" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK45" s="12">
         <v>750</v>
       </c>
-      <c r="AK45" s="12">
+      <c r="AL45" s="12">
         <v>14876</v>
       </c>
-      <c r="AL45" s="12">
+      <c r="AM45" s="12">
         <v>28350</v>
       </c>
-      <c r="AM45" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN45" s="12">
-        <v>0</v>
+      <c r="AN45" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="AO45" s="12">
         <v>0</v>
       </c>
       <c r="AP45" s="12">
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="12">
         <v>9403</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>114</v>
       </c>
@@ -6810,9 +6902,7 @@
       <c r="AA46" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB46" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB46" s="12"/>
       <c r="AC46" s="12" t="s">
         <v>87</v>
       </c>
@@ -6834,29 +6924,32 @@
       <c r="AI46" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AJ46" s="12">
+      <c r="AJ46" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK46" s="12">
         <v>78</v>
       </c>
-      <c r="AK46" s="12">
+      <c r="AL46" s="12">
         <v>40</v>
       </c>
-      <c r="AL46" s="12">
+      <c r="AM46" s="12">
         <v>97</v>
       </c>
-      <c r="AM46" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN46" s="12">
+      <c r="AN46" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO46" s="12">
         <v>498</v>
       </c>
-      <c r="AO46" s="12">
+      <c r="AP46" s="12">
         <v>693</v>
       </c>
-      <c r="AP46" s="12">
+      <c r="AQ46" s="12">
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>114</v>
       </c>
@@ -6936,9 +7029,7 @@
       <c r="AA47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB47" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB47" s="12"/>
       <c r="AC47" s="12" t="s">
         <v>87</v>
       </c>
@@ -6963,26 +7054,29 @@
       <c r="AJ47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AK47" s="12">
+      <c r="AK47" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL47" s="12">
         <v>669</v>
       </c>
-      <c r="AL47" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AM47" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AN47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AO47" s="12">
+      <c r="AO47" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP47" s="12">
         <v>16172</v>
       </c>
-      <c r="AP47" s="12" t="s">
+      <c r="AQ47" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
         <v>115</v>
       </c>
@@ -7062,30 +7156,28 @@
       <c r="AA48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB48" s="12">
+      <c r="AB48" s="12"/>
+      <c r="AC48" s="12">
         <v>50</v>
       </c>
-      <c r="AC48" s="12">
+      <c r="AD48" s="12">
         <v>200</v>
       </c>
-      <c r="AD48" s="12">
+      <c r="AE48" s="12">
         <v>225</v>
       </c>
-      <c r="AE48" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF48" s="12">
+      <c r="AF48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG48" s="12">
         <v>100</v>
       </c>
-      <c r="AG48" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH48" s="12">
+      <c r="AH48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI48" s="12">
         <v>500</v>
       </c>
-      <c r="AI48" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AJ48" s="12" t="s">
         <v>87</v>
       </c>
@@ -7095,20 +7187,23 @@
       <c r="AL48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AM48" s="12">
+      <c r="AM48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN48" s="12">
         <v>0</v>
       </c>
-      <c r="AN48" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AO48" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AP48" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ48" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>115</v>
       </c>
@@ -7188,9 +7283,7 @@
       <c r="AA49" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB49" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB49" s="12"/>
       <c r="AC49" s="12" t="s">
         <v>87</v>
       </c>
@@ -7233,8 +7326,11 @@
       <c r="AP49" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ49" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>116</v>
       </c>
@@ -7314,27 +7410,25 @@
       <c r="AA50" s="12">
         <v>-69</v>
       </c>
-      <c r="AB50" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB50" s="12"/>
       <c r="AC50" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AD50" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AE50" s="12">
+      <c r="AE50" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF50" s="12">
         <v>-50</v>
       </c>
-      <c r="AF50" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG50" s="12">
+      <c r="AG50" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH50" s="12">
         <v>-150</v>
       </c>
-      <c r="AH50" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI50" s="12" t="s">
         <v>87</v>
       </c>
@@ -7359,8 +7453,11 @@
       <c r="AP50" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ50" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>117</v>
       </c>
@@ -7440,9 +7537,7 @@
       <c r="AA51" s="12">
         <v>-725</v>
       </c>
-      <c r="AB51" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB51" s="12"/>
       <c r="AC51" s="12" t="s">
         <v>87</v>
       </c>
@@ -7485,8 +7580,11 @@
       <c r="AP51" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ51" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>118</v>
       </c>
@@ -7566,53 +7664,54 @@
       <c r="AA52" s="12">
         <v>-1142</v>
       </c>
-      <c r="AB52" s="12">
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="12">
         <v>-64</v>
       </c>
-      <c r="AC52" s="12">
+      <c r="AD52" s="12">
         <v>-78</v>
       </c>
-      <c r="AD52" s="12">
+      <c r="AE52" s="12">
         <v>-102</v>
       </c>
-      <c r="AE52" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF52" s="12">
+      <c r="AF52" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG52" s="12">
         <v>-34</v>
       </c>
-      <c r="AG52" s="12">
+      <c r="AH52" s="12">
         <v>-38</v>
       </c>
-      <c r="AH52" s="12">
+      <c r="AI52" s="12">
         <v>-252</v>
       </c>
-      <c r="AI52" s="12">
+      <c r="AJ52" s="12">
         <v>-662</v>
       </c>
-      <c r="AJ52" s="12">
+      <c r="AK52" s="12">
         <v>-101</v>
       </c>
-      <c r="AK52" s="12">
+      <c r="AL52" s="12">
         <v>-42</v>
       </c>
-      <c r="AL52" s="12">
+      <c r="AM52" s="12">
         <v>-130</v>
       </c>
-      <c r="AM52" s="12">
+      <c r="AN52" s="12">
         <v>-14</v>
       </c>
-      <c r="AN52" s="12">
+      <c r="AO52" s="12">
         <v>-1250</v>
       </c>
-      <c r="AO52" s="12">
+      <c r="AP52" s="12">
         <v>-184</v>
       </c>
-      <c r="AP52" s="12">
+      <c r="AQ52" s="12">
         <v>-18</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>119</v>
       </c>
@@ -7692,53 +7791,54 @@
       <c r="AA53" s="12">
         <v>316</v>
       </c>
-      <c r="AB53" s="12">
+      <c r="AB53" s="12"/>
+      <c r="AC53" s="12">
         <v>-1120</v>
       </c>
-      <c r="AC53" s="12">
+      <c r="AD53" s="12">
         <v>1036</v>
       </c>
-      <c r="AD53" s="12">
+      <c r="AE53" s="12">
         <v>572</v>
       </c>
-      <c r="AE53" s="12">
+      <c r="AF53" s="12">
         <v>-838</v>
       </c>
-      <c r="AF53" s="12">
+      <c r="AG53" s="12">
         <v>-257</v>
       </c>
-      <c r="AG53" s="12">
+      <c r="AH53" s="12">
         <v>-106</v>
       </c>
-      <c r="AH53" s="12">
+      <c r="AI53" s="12">
         <v>-2065</v>
       </c>
-      <c r="AI53" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AJ53" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AK53" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AL53" s="12">
-        <v>0</v>
+      <c r="AL53" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="AM53" s="12">
         <v>0</v>
       </c>
-      <c r="AN53" s="12" t="s">
-        <v>87</v>
+      <c r="AN53" s="12">
+        <v>0</v>
       </c>
       <c r="AO53" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AP53" s="12">
+      <c r="AP53" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ53" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>120</v>
       </c>
@@ -7818,9 +7918,7 @@
       <c r="AA54" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB54" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB54" s="12"/>
       <c r="AC54" s="12" t="s">
         <v>87</v>
       </c>
@@ -7863,8 +7961,11 @@
       <c r="AP54" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ54" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>121</v>
       </c>
@@ -7944,21 +8045,19 @@
       <c r="AA55" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB55" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB55" s="12"/>
       <c r="AC55" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AD55" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AE55" s="12">
+      <c r="AE55" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF55" s="12">
         <v>8</v>
       </c>
-      <c r="AF55" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG55" s="12" t="s">
         <v>87</v>
       </c>
@@ -7989,8 +8088,11 @@
       <c r="AP55" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ55" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>122</v>
       </c>
@@ -8070,21 +8172,19 @@
       <c r="AA56" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB56" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB56" s="12"/>
       <c r="AC56" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AD56" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AE56" s="12">
+      <c r="AE56" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF56" s="12">
         <v>5</v>
       </c>
-      <c r="AF56" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG56" s="12" t="s">
         <v>87</v>
       </c>
@@ -8103,20 +8203,23 @@
       <c r="AL56" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AM56" s="12">
+      <c r="AM56" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN56" s="12">
         <v>318</v>
       </c>
-      <c r="AN56" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AO56" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AP56" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ56" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
         <v>123</v>
       </c>
@@ -8196,53 +8299,54 @@
       <c r="AA57" s="12">
         <v>13045</v>
       </c>
-      <c r="AB57" s="12">
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="12">
         <v>10389</v>
       </c>
-      <c r="AC57" s="12">
+      <c r="AD57" s="12">
         <v>17197</v>
       </c>
-      <c r="AD57" s="12">
+      <c r="AE57" s="12">
         <v>19274</v>
       </c>
-      <c r="AE57" s="12">
+      <c r="AF57" s="12">
         <v>16045</v>
       </c>
-      <c r="AF57" s="12">
+      <c r="AG57" s="12">
         <v>17443</v>
       </c>
-      <c r="AG57" s="12">
+      <c r="AH57" s="12">
         <v>20346</v>
       </c>
-      <c r="AH57" s="12">
+      <c r="AI57" s="12">
         <v>16590</v>
       </c>
-      <c r="AI57" s="12">
+      <c r="AJ57" s="12">
         <v>12516</v>
       </c>
-      <c r="AJ57" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK57" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AL57" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AM57" s="12">
+      <c r="AM57" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN57" s="12">
         <v>11371</v>
       </c>
-      <c r="AN57" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AO57" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AP57" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ57" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>123</v>
       </c>
@@ -8322,9 +8426,7 @@
       <c r="AA58" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB58" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB58" s="12"/>
       <c r="AC58" s="12" t="s">
         <v>87</v>
       </c>
@@ -8346,29 +8448,32 @@
       <c r="AI58" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AJ58" s="12">
+      <c r="AJ58" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK58" s="12">
         <v>19362</v>
       </c>
-      <c r="AK58" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AL58" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AM58" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AN58" s="12">
+      <c r="AN58" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO58" s="12">
         <v>9351</v>
       </c>
-      <c r="AO58" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AP58" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ58" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
         <v>124</v>
       </c>
@@ -8448,53 +8553,54 @@
       <c r="AA59" s="12">
         <v>-18335</v>
       </c>
-      <c r="AB59" s="12">
+      <c r="AB59" s="12"/>
+      <c r="AC59" s="12">
         <v>-12558</v>
       </c>
-      <c r="AC59" s="12">
+      <c r="AD59" s="12">
         <v>-20568</v>
       </c>
-      <c r="AD59" s="12">
+      <c r="AE59" s="12">
         <v>-23091</v>
       </c>
-      <c r="AE59" s="12">
+      <c r="AF59" s="12">
         <v>-18151</v>
       </c>
-      <c r="AF59" s="12">
+      <c r="AG59" s="12">
         <v>-20748</v>
       </c>
-      <c r="AG59" s="12">
+      <c r="AH59" s="12">
         <v>-24840</v>
       </c>
-      <c r="AH59" s="12">
+      <c r="AI59" s="12">
         <v>-25371</v>
       </c>
-      <c r="AI59" s="12">
+      <c r="AJ59" s="12">
         <v>-13550</v>
       </c>
-      <c r="AJ59" s="12">
+      <c r="AK59" s="12">
         <v>-20119</v>
       </c>
-      <c r="AK59" s="12">
+      <c r="AL59" s="12">
         <v>-19557</v>
       </c>
-      <c r="AL59" s="12">
+      <c r="AM59" s="12">
         <v>-39033</v>
       </c>
-      <c r="AM59" s="12">
+      <c r="AN59" s="12">
         <v>-13486</v>
       </c>
-      <c r="AN59" s="12">
+      <c r="AO59" s="12">
         <v>-8849</v>
       </c>
-      <c r="AO59" s="12">
+      <c r="AP59" s="12">
         <v>-14192</v>
       </c>
-      <c r="AP59" s="12">
+      <c r="AQ59" s="12">
         <v>-14299</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
         <v>125</v>
       </c>
@@ -8574,9 +8680,7 @@
       <c r="AA60" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB60" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB60" s="12"/>
       <c r="AC60" s="12" t="s">
         <v>87</v>
       </c>
@@ -8619,8 +8723,11 @@
       <c r="AP60" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ60" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>126</v>
       </c>
@@ -8700,53 +8807,54 @@
       <c r="AA61" s="14">
         <v>-9327</v>
       </c>
-      <c r="AB61" s="14">
+      <c r="AB61" s="14"/>
+      <c r="AC61" s="14">
         <v>-7304</v>
       </c>
-      <c r="AC61" s="14">
+      <c r="AD61" s="14">
         <v>-5103</v>
       </c>
-      <c r="AD61" s="14">
+      <c r="AE61" s="14">
         <v>-5817</v>
       </c>
-      <c r="AE61" s="14">
+      <c r="AF61" s="14">
         <v>-5487</v>
       </c>
-      <c r="AF61" s="14">
+      <c r="AG61" s="14">
         <v>-6245</v>
       </c>
-      <c r="AG61" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH61" s="14">
+      <c r="AH61" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI61" s="14">
         <v>-13045</v>
       </c>
-      <c r="AI61" s="14">
+      <c r="AJ61" s="14">
         <v>-4702</v>
       </c>
-      <c r="AJ61" s="14">
+      <c r="AK61" s="14">
         <v>-2851</v>
       </c>
-      <c r="AK61" s="14">
+      <c r="AL61" s="14">
         <v>-7172</v>
       </c>
-      <c r="AL61" s="14">
+      <c r="AM61" s="14">
         <v>-14404</v>
       </c>
-      <c r="AM61" s="14">
+      <c r="AN61" s="14">
         <v>-6974</v>
       </c>
-      <c r="AN61" s="14">
+      <c r="AO61" s="14">
         <v>-7846</v>
       </c>
-      <c r="AO61" s="14">
+      <c r="AP61" s="14">
         <v>-3374</v>
       </c>
-      <c r="AP61" s="14">
+      <c r="AQ61" s="14">
         <v>-10408</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>126</v>
       </c>
@@ -8826,9 +8934,7 @@
       <c r="AA62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AB62" s="14" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB62" s="14"/>
       <c r="AC62" s="14" t="s">
         <v>87</v>
       </c>
@@ -8841,12 +8947,12 @@
       <c r="AF62" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AG62" s="14">
+      <c r="AG62" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH62" s="14">
         <v>-7173</v>
       </c>
-      <c r="AH62" s="14" t="s">
-        <v>87</v>
-      </c>
       <c r="AI62" s="14" t="s">
         <v>87</v>
       </c>
@@ -8871,8 +8977,11 @@
       <c r="AP62" s="14" t="s">
         <v>87</v>
       </c>
+      <c r="AQ62" s="14" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
         <v>127</v>
       </c>
@@ -8917,8 +9026,9 @@
       <c r="AN63" s="11"/>
       <c r="AO63" s="11"/>
       <c r="AP63" s="11"/>
+      <c r="AQ63" s="11"/>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>128</v>
       </c>
@@ -8998,9 +9108,7 @@
       <c r="AA64" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB64" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB64" s="12"/>
       <c r="AC64" s="12" t="s">
         <v>87</v>
       </c>
@@ -9043,8 +9151,11 @@
       <c r="AP64" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ64" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
         <v>129</v>
       </c>
@@ -9124,9 +9235,7 @@
       <c r="AA65" s="12">
         <v>2874</v>
       </c>
-      <c r="AB65" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB65" s="12"/>
       <c r="AC65" s="12" t="s">
         <v>87</v>
       </c>
@@ -9169,8 +9278,11 @@
       <c r="AP65" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ65" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
         <v>130</v>
       </c>
@@ -9250,9 +9362,7 @@
       <c r="AA66" s="12">
         <v>-2877</v>
       </c>
-      <c r="AB66" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB66" s="12"/>
       <c r="AC66" s="12" t="s">
         <v>87</v>
       </c>
@@ -9295,8 +9405,11 @@
       <c r="AP66" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ66" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
         <v>131</v>
       </c>
@@ -9376,9 +9489,7 @@
       <c r="AA67" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB67" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB67" s="12"/>
       <c r="AC67" s="12" t="s">
         <v>87</v>
       </c>
@@ -9421,8 +9532,11 @@
       <c r="AP67" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ67" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
         <v>132</v>
       </c>
@@ -9502,9 +9616,7 @@
       <c r="AA68" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB68" s="12">
-        <v>0</v>
-      </c>
+      <c r="AB68" s="12"/>
       <c r="AC68" s="12">
         <v>0</v>
       </c>
@@ -9512,43 +9624,46 @@
         <v>0</v>
       </c>
       <c r="AE68" s="12">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="12">
         <v>-1780</v>
       </c>
-      <c r="AF68" s="12">
+      <c r="AG68" s="12">
         <v>-2098</v>
       </c>
-      <c r="AG68" s="12">
+      <c r="AH68" s="12">
         <v>-1595</v>
       </c>
-      <c r="AH68" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI68" s="12">
+      <c r="AI68" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ68" s="12">
         <v>0</v>
       </c>
-      <c r="AJ68" s="12">
+      <c r="AK68" s="12">
         <v>-1127</v>
       </c>
-      <c r="AK68" s="12">
+      <c r="AL68" s="12">
         <v>-1618</v>
       </c>
-      <c r="AL68" s="12">
+      <c r="AM68" s="12">
         <v>0</v>
       </c>
-      <c r="AM68" s="12">
+      <c r="AN68" s="12">
         <v>-2101</v>
       </c>
-      <c r="AN68" s="12">
+      <c r="AO68" s="12">
         <v>-2173</v>
       </c>
-      <c r="AO68" s="12">
+      <c r="AP68" s="12">
         <v>-2052</v>
       </c>
-      <c r="AP68" s="12">
+      <c r="AQ68" s="12">
         <v>-2200</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
         <v>133</v>
       </c>
@@ -9628,53 +9743,54 @@
       <c r="AA69" s="12">
         <v>-227</v>
       </c>
-      <c r="AB69" s="12">
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="12">
         <v>-293</v>
       </c>
-      <c r="AC69" s="12">
+      <c r="AD69" s="12">
         <v>45</v>
       </c>
-      <c r="AD69" s="12">
+      <c r="AE69" s="12">
         <v>-104</v>
       </c>
-      <c r="AE69" s="12">
+      <c r="AF69" s="12">
         <v>-82</v>
       </c>
-      <c r="AF69" s="12">
+      <c r="AG69" s="12">
         <v>60</v>
       </c>
-      <c r="AG69" s="12">
+      <c r="AH69" s="12">
         <v>9</v>
       </c>
-      <c r="AH69" s="12">
+      <c r="AI69" s="12">
         <v>68</v>
       </c>
-      <c r="AI69" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ69" s="12">
+      <c r="AJ69" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK69" s="12">
         <v>191</v>
       </c>
-      <c r="AK69" s="12">
+      <c r="AL69" s="12">
         <v>88</v>
       </c>
-      <c r="AL69" s="12">
+      <c r="AM69" s="12">
         <v>108</v>
       </c>
-      <c r="AM69" s="12">
+      <c r="AN69" s="12">
         <v>18</v>
       </c>
-      <c r="AN69" s="12">
+      <c r="AO69" s="12">
         <v>165</v>
       </c>
-      <c r="AO69" s="12">
+      <c r="AP69" s="12">
         <v>-331</v>
       </c>
-      <c r="AP69" s="12">
+      <c r="AQ69" s="12">
         <v>-29</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
         <v>133</v>
       </c>
@@ -9754,9 +9870,7 @@
       <c r="AA70" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB70" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB70" s="12"/>
       <c r="AC70" s="12" t="s">
         <v>87</v>
       </c>
@@ -9775,12 +9889,12 @@
       <c r="AH70" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI70" s="12">
+      <c r="AI70" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ70" s="12">
         <v>-307</v>
       </c>
-      <c r="AJ70" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK70" s="12" t="s">
         <v>87</v>
       </c>
@@ -9799,8 +9913,11 @@
       <c r="AP70" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ70" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
         <v>134</v>
       </c>
@@ -9880,9 +9997,7 @@
       <c r="AA71" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB71" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB71" s="12"/>
       <c r="AC71" s="12" t="s">
         <v>87</v>
       </c>
@@ -9904,29 +10019,32 @@
       <c r="AI71" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AJ71" s="12">
+      <c r="AJ71" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK71" s="12">
         <v>0</v>
       </c>
-      <c r="AK71" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AL71" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AM71" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AN71" s="12">
+      <c r="AN71" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO71" s="12">
         <v>4691</v>
       </c>
-      <c r="AO71" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AP71" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ71" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
         <v>135</v>
       </c>
@@ -10006,53 +10124,54 @@
       <c r="AA72" s="12">
         <v>-627</v>
       </c>
-      <c r="AB72" s="12">
+      <c r="AB72" s="12"/>
+      <c r="AC72" s="12">
         <v>-493</v>
       </c>
-      <c r="AC72" s="12">
+      <c r="AD72" s="12">
         <v>-511</v>
       </c>
-      <c r="AD72" s="12">
+      <c r="AE72" s="12">
         <v>-606</v>
       </c>
-      <c r="AE72" s="12">
+      <c r="AF72" s="12">
         <v>-765</v>
       </c>
-      <c r="AF72" s="12">
+      <c r="AG72" s="12">
         <v>-807</v>
       </c>
-      <c r="AG72" s="12">
+      <c r="AH72" s="12">
         <v>-803</v>
       </c>
-      <c r="AH72" s="12">
+      <c r="AI72" s="12">
         <v>-815</v>
       </c>
-      <c r="AI72" s="12">
+      <c r="AJ72" s="12">
         <v>-879</v>
       </c>
-      <c r="AJ72" s="12">
+      <c r="AK72" s="12">
         <v>-1009</v>
       </c>
-      <c r="AK72" s="12">
+      <c r="AL72" s="12">
         <v>-1084</v>
       </c>
-      <c r="AL72" s="12">
+      <c r="AM72" s="12">
         <v>-1018</v>
       </c>
-      <c r="AM72" s="12">
+      <c r="AN72" s="12">
         <v>-1055</v>
       </c>
-      <c r="AN72" s="12">
+      <c r="AO72" s="12">
         <v>-1158</v>
       </c>
-      <c r="AO72" s="12">
+      <c r="AP72" s="12">
         <v>-1541</v>
       </c>
-      <c r="AP72" s="12">
+      <c r="AQ72" s="12">
         <v>-1253</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
         <v>135</v>
       </c>
@@ -10132,41 +10251,39 @@
       <c r="AA73" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB73" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC73" s="12">
+      <c r="AB73" s="12"/>
+      <c r="AC73" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD73" s="12">
         <v>-47</v>
       </c>
-      <c r="AD73" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE73" s="12">
+      <c r="AE73" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF73" s="12">
         <v>0</v>
       </c>
-      <c r="AF73" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG73" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AH73" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI73" s="12">
+      <c r="AI73" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ73" s="12">
         <v>0</v>
       </c>
-      <c r="AJ73" s="12">
+      <c r="AK73" s="12">
         <v>480</v>
       </c>
-      <c r="AK73" s="12">
+      <c r="AL73" s="12">
         <v>0</v>
       </c>
-      <c r="AL73" s="12">
+      <c r="AM73" s="12">
         <v>320</v>
-      </c>
-      <c r="AM73" s="12">
-        <v>0</v>
       </c>
       <c r="AN73" s="12">
         <v>0</v>
@@ -10177,8 +10294,11 @@
       <c r="AP73" s="12">
         <v>0</v>
       </c>
+      <c r="AQ73" s="12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>136</v>
       </c>
@@ -10258,33 +10378,31 @@
       <c r="AA74" s="12">
         <v>2382</v>
       </c>
-      <c r="AB74" s="12">
+      <c r="AB74" s="12"/>
+      <c r="AC74" s="12">
         <v>98</v>
       </c>
-      <c r="AC74" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD74" s="12">
+      <c r="AD74" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE74" s="12">
         <v>2543</v>
       </c>
-      <c r="AE74" s="12">
+      <c r="AF74" s="12">
         <v>3651</v>
       </c>
-      <c r="AF74" s="12">
+      <c r="AG74" s="12">
         <v>166</v>
       </c>
-      <c r="AG74" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH74" s="12">
+      <c r="AH74" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI74" s="12">
         <v>934</v>
       </c>
-      <c r="AI74" s="12">
+      <c r="AJ74" s="12">
         <v>-934</v>
       </c>
-      <c r="AJ74" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK74" s="12" t="s">
         <v>87</v>
       </c>
@@ -10303,8 +10421,11 @@
       <c r="AP74" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ74" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
         <v>136</v>
       </c>
@@ -10384,33 +10505,31 @@
       <c r="AA75" s="12">
         <v>1666</v>
       </c>
-      <c r="AB75" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB75" s="12"/>
       <c r="AC75" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD75" s="12">
+      <c r="AD75" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE75" s="12">
         <v>234</v>
       </c>
-      <c r="AE75" s="12">
+      <c r="AF75" s="12">
         <v>-2543</v>
       </c>
-      <c r="AF75" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG75" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AH75" s="12">
+      <c r="AH75" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI75" s="12">
         <v>24</v>
       </c>
-      <c r="AI75" s="12">
+      <c r="AJ75" s="12">
         <v>1643</v>
       </c>
-      <c r="AJ75" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK75" s="12" t="s">
         <v>87</v>
       </c>
@@ -10429,8 +10548,11 @@
       <c r="AP75" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ75" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
         <v>137</v>
       </c>
@@ -10510,33 +10632,31 @@
       <c r="AA76" s="12">
         <v>56</v>
       </c>
-      <c r="AB76" s="12">
+      <c r="AB76" s="12"/>
+      <c r="AC76" s="12">
         <v>18</v>
       </c>
-      <c r="AC76" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AD76" s="12">
+      <c r="AD76" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE76" s="12">
         <v>66</v>
       </c>
-      <c r="AE76" s="12">
+      <c r="AF76" s="12">
         <v>96</v>
       </c>
-      <c r="AF76" s="12">
+      <c r="AG76" s="12">
         <v>18</v>
       </c>
-      <c r="AG76" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH76" s="12">
+      <c r="AH76" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI76" s="12">
         <v>66</v>
       </c>
-      <c r="AI76" s="12">
+      <c r="AJ76" s="12">
         <v>-66</v>
       </c>
-      <c r="AJ76" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK76" s="12" t="s">
         <v>87</v>
       </c>
@@ -10555,8 +10675,11 @@
       <c r="AP76" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ76" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
         <v>137</v>
       </c>
@@ -10636,33 +10759,31 @@
       <c r="AA77" s="12">
         <v>38</v>
       </c>
-      <c r="AB77" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB77" s="12"/>
       <c r="AC77" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AD77" s="12">
+      <c r="AD77" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE77" s="12">
         <v>48</v>
       </c>
-      <c r="AE77" s="12">
+      <c r="AF77" s="12">
         <v>-66</v>
       </c>
-      <c r="AF77" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AG77" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AH77" s="12">
+      <c r="AH77" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI77" s="12">
         <v>-48</v>
       </c>
-      <c r="AI77" s="12">
+      <c r="AJ77" s="12">
         <v>84</v>
       </c>
-      <c r="AJ77" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK77" s="12" t="s">
         <v>87</v>
       </c>
@@ -10681,8 +10802,11 @@
       <c r="AP77" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ77" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
         <v>138</v>
       </c>
@@ -10762,9 +10886,7 @@
       <c r="AA78" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB78" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB78" s="12"/>
       <c r="AC78" s="12" t="s">
         <v>87</v>
       </c>
@@ -10807,8 +10929,11 @@
       <c r="AP78" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ78" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
         <v>139</v>
       </c>
@@ -10888,53 +11013,54 @@
       <c r="AA79" s="12">
         <v>-4015</v>
       </c>
-      <c r="AB79" s="12">
+      <c r="AB79" s="12"/>
+      <c r="AC79" s="12">
         <v>-1371</v>
       </c>
-      <c r="AC79" s="12">
+      <c r="AD79" s="12">
         <v>1477</v>
       </c>
-      <c r="AD79" s="12">
+      <c r="AE79" s="12">
         <v>-385</v>
       </c>
-      <c r="AE79" s="12">
+      <c r="AF79" s="12">
         <v>-1519</v>
       </c>
-      <c r="AF79" s="12">
+      <c r="AG79" s="12">
         <v>-1438</v>
       </c>
-      <c r="AG79" s="12">
+      <c r="AH79" s="12">
         <v>-1484</v>
       </c>
-      <c r="AH79" s="12">
+      <c r="AI79" s="12">
         <v>-4221</v>
       </c>
-      <c r="AI79" s="12">
+      <c r="AJ79" s="12">
         <v>3512</v>
       </c>
-      <c r="AJ79" s="12">
+      <c r="AK79" s="12">
         <v>5214</v>
       </c>
-      <c r="AK79" s="12">
+      <c r="AL79" s="12">
         <v>-2421</v>
       </c>
-      <c r="AL79" s="12">
+      <c r="AM79" s="12">
         <v>-5130</v>
       </c>
-      <c r="AM79" s="12">
+      <c r="AN79" s="12">
         <v>134</v>
       </c>
-      <c r="AN79" s="12">
+      <c r="AO79" s="12">
         <v>1943</v>
       </c>
-      <c r="AO79" s="12">
+      <c r="AP79" s="12">
         <v>1490</v>
       </c>
-      <c r="AP79" s="12">
+      <c r="AQ79" s="12">
         <v>-705</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
         <v>140</v>
       </c>
@@ -11014,53 +11140,54 @@
       <c r="AA80" s="12">
         <v>15605</v>
       </c>
-      <c r="AB80" s="12">
+      <c r="AB80" s="12"/>
+      <c r="AC80" s="12">
         <v>16976</v>
       </c>
-      <c r="AC80" s="12">
+      <c r="AD80" s="12">
         <v>18453</v>
       </c>
-      <c r="AD80" s="12">
+      <c r="AE80" s="12">
         <v>18068</v>
       </c>
-      <c r="AE80" s="12">
+      <c r="AF80" s="12">
         <v>16549</v>
       </c>
-      <c r="AF80" s="12">
+      <c r="AG80" s="12">
         <v>15111</v>
       </c>
-      <c r="AG80" s="12">
+      <c r="AH80" s="12">
         <v>13627</v>
       </c>
-      <c r="AH80" s="12">
+      <c r="AI80" s="12">
         <v>9406</v>
       </c>
-      <c r="AI80" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ80" s="12">
+      <c r="AJ80" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK80" s="12">
         <v>18132</v>
       </c>
-      <c r="AK80" s="12">
+      <c r="AL80" s="12">
         <v>15711</v>
       </c>
-      <c r="AL80" s="12">
+      <c r="AM80" s="12">
         <v>10581</v>
       </c>
-      <c r="AM80" s="12">
+      <c r="AN80" s="12">
         <v>10715</v>
       </c>
-      <c r="AN80" s="12">
+      <c r="AO80" s="12">
         <v>12658</v>
       </c>
-      <c r="AO80" s="12">
+      <c r="AP80" s="12">
         <v>14148</v>
       </c>
-      <c r="AP80" s="12">
+      <c r="AQ80" s="12">
         <v>13443</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>140</v>
       </c>
@@ -11140,9 +11267,7 @@
       <c r="AA81" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB81" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB81" s="12"/>
       <c r="AC81" s="12" t="s">
         <v>87</v>
       </c>
@@ -11161,12 +11286,12 @@
       <c r="AH81" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AI81" s="12">
+      <c r="AI81" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ81" s="12">
         <v>12918</v>
       </c>
-      <c r="AJ81" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AK81" s="12" t="s">
         <v>87</v>
       </c>
@@ -11185,8 +11310,11 @@
       <c r="AP81" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ81" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
         <v>141</v>
       </c>
@@ -11266,53 +11394,54 @@
       <c r="AA82" s="12">
         <v>19620</v>
       </c>
-      <c r="AB82" s="12">
+      <c r="AB82" s="12"/>
+      <c r="AC82" s="12">
         <v>18347</v>
       </c>
-      <c r="AC82" s="12">
+      <c r="AD82" s="12">
         <v>16976</v>
       </c>
-      <c r="AD82" s="12">
+      <c r="AE82" s="12">
         <v>18453</v>
       </c>
-      <c r="AE82" s="12">
+      <c r="AF82" s="12">
         <v>18068</v>
       </c>
-      <c r="AF82" s="12">
+      <c r="AG82" s="12">
         <v>16549</v>
       </c>
-      <c r="AG82" s="12">
+      <c r="AH82" s="12">
         <v>15111</v>
       </c>
-      <c r="AH82" s="12">
+      <c r="AI82" s="12">
         <v>13627</v>
       </c>
-      <c r="AI82" s="12">
+      <c r="AJ82" s="12">
         <v>9406</v>
       </c>
-      <c r="AJ82" s="12">
+      <c r="AK82" s="12">
         <v>12918</v>
       </c>
-      <c r="AK82" s="12">
+      <c r="AL82" s="12">
         <v>18132</v>
       </c>
-      <c r="AL82" s="12">
+      <c r="AM82" s="12">
         <v>15711</v>
       </c>
-      <c r="AM82" s="12">
+      <c r="AN82" s="12">
         <v>10581</v>
       </c>
-      <c r="AN82" s="12">
+      <c r="AO82" s="12">
         <v>10715</v>
       </c>
-      <c r="AO82" s="12">
+      <c r="AP82" s="12">
         <v>12658</v>
       </c>
-      <c r="AP82" s="12">
+      <c r="AQ82" s="12">
         <v>14148</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
         <v>142</v>
       </c>
@@ -11392,53 +11521,54 @@
       <c r="AA83" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB83" s="12">
+      <c r="AB83" s="12"/>
+      <c r="AC83" s="12">
         <v>-3308</v>
       </c>
-      <c r="AC83" s="12">
+      <c r="AD83" s="12">
         <v>-3396</v>
       </c>
-      <c r="AD83" s="12">
+      <c r="AE83" s="12">
         <v>-3637</v>
       </c>
-      <c r="AE83" s="12">
+      <c r="AF83" s="12">
         <v>-3387</v>
       </c>
-      <c r="AF83" s="12">
+      <c r="AG83" s="12">
         <v>-3962</v>
       </c>
-      <c r="AG83" s="12">
+      <c r="AH83" s="12">
         <v>-2839</v>
       </c>
-      <c r="AH83" s="12">
+      <c r="AI83" s="12">
         <v>-3250</v>
       </c>
-      <c r="AI83" s="12">
+      <c r="AJ83" s="12">
         <v>-13</v>
       </c>
-      <c r="AJ83" s="12">
+      <c r="AK83" s="12">
         <v>-18</v>
       </c>
-      <c r="AK83" s="12">
+      <c r="AL83" s="12">
         <v>-38</v>
       </c>
-      <c r="AL83" s="12">
+      <c r="AM83" s="12">
         <v>-2706</v>
       </c>
-      <c r="AM83" s="12">
+      <c r="AN83" s="12">
         <v>-1615</v>
       </c>
-      <c r="AN83" s="12">
+      <c r="AO83" s="12">
         <v>-3378</v>
       </c>
-      <c r="AO83" s="12">
+      <c r="AP83" s="12">
         <v>-2889</v>
       </c>
-      <c r="AP83" s="12">
+      <c r="AQ83" s="12">
         <v>-555</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
         <v>134</v>
       </c>
@@ -11518,53 +11648,54 @@
       <c r="AA84" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB84" s="12">
+      <c r="AB84" s="12"/>
+      <c r="AC84" s="12">
         <v>3305</v>
       </c>
-      <c r="AC84" s="12">
+      <c r="AD84" s="12">
         <v>3393</v>
       </c>
-      <c r="AD84" s="12">
+      <c r="AE84" s="12">
         <v>3634</v>
       </c>
-      <c r="AE84" s="12">
+      <c r="AF84" s="12">
         <v>3373</v>
       </c>
-      <c r="AF84" s="12">
+      <c r="AG84" s="12">
         <v>3956</v>
       </c>
-      <c r="AG84" s="12">
+      <c r="AH84" s="12">
         <v>1797</v>
       </c>
-      <c r="AH84" s="12">
+      <c r="AI84" s="12">
         <v>2976</v>
       </c>
-      <c r="AI84" s="12">
+      <c r="AJ84" s="12">
         <v>0</v>
       </c>
-      <c r="AJ84" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK84" s="12">
+      <c r="AK84" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL84" s="12">
         <v>0</v>
       </c>
-      <c r="AL84" s="12">
+      <c r="AM84" s="12">
         <v>2698</v>
       </c>
-      <c r="AM84" s="12">
+      <c r="AN84" s="12">
         <v>1593</v>
       </c>
-      <c r="AN84" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO84" s="12">
+      <c r="AO84" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP84" s="12">
         <v>1545</v>
       </c>
-      <c r="AP84" s="12">
+      <c r="AQ84" s="12">
         <v>530</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
         <v>143</v>
       </c>
@@ -11644,9 +11775,7 @@
       <c r="AA85" s="12">
         <v>175</v>
       </c>
-      <c r="AB85" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB85" s="12"/>
       <c r="AC85" s="12" t="s">
         <v>87</v>
       </c>
@@ -11689,8 +11818,11 @@
       <c r="AP85" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ85" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>144</v>
       </c>
@@ -11770,53 +11902,54 @@
       <c r="AA86" s="14">
         <v>-455</v>
       </c>
-      <c r="AB86" s="14">
+      <c r="AB86" s="14"/>
+      <c r="AC86" s="14">
         <v>-496</v>
       </c>
-      <c r="AC86" s="14">
+      <c r="AD86" s="14">
         <v>-561</v>
       </c>
-      <c r="AD86" s="14">
+      <c r="AE86" s="14">
         <v>-609</v>
       </c>
-      <c r="AE86" s="14">
+      <c r="AF86" s="14">
         <v>-2559</v>
       </c>
-      <c r="AF86" s="14">
+      <c r="AG86" s="14">
         <v>-2911</v>
       </c>
-      <c r="AG86" s="14">
+      <c r="AH86" s="14">
         <v>-3440</v>
       </c>
-      <c r="AH86" s="14">
+      <c r="AI86" s="14">
         <v>-1089</v>
       </c>
-      <c r="AI86" s="14">
+      <c r="AJ86" s="14">
         <v>-892</v>
       </c>
-      <c r="AJ86" s="14">
+      <c r="AK86" s="14">
         <v>-1674</v>
       </c>
-      <c r="AK86" s="14">
+      <c r="AL86" s="14">
         <v>-2740</v>
       </c>
-      <c r="AL86" s="14">
+      <c r="AM86" s="14">
         <v>-706</v>
       </c>
-      <c r="AM86" s="14">
+      <c r="AN86" s="14">
         <v>-3178</v>
       </c>
-      <c r="AN86" s="14">
+      <c r="AO86" s="14">
         <v>-2018</v>
       </c>
-      <c r="AO86" s="14">
+      <c r="AP86" s="14">
         <v>-4937</v>
       </c>
-      <c r="AP86" s="14">
+      <c r="AQ86" s="14">
         <v>-3478</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
         <v>145</v>
       </c>
@@ -11861,8 +11994,9 @@
       <c r="AN87" s="11"/>
       <c r="AO87" s="11"/>
       <c r="AP87" s="11"/>
+      <c r="AQ87" s="11"/>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
         <v>136</v>
       </c>
@@ -11942,27 +12076,25 @@
       <c r="AA88" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB88" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC88" s="12">
+      <c r="AB88" s="12"/>
+      <c r="AC88" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD88" s="12">
         <v>98</v>
       </c>
-      <c r="AD88" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AE88" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AF88" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG88" s="12">
+      <c r="AG88" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH88" s="12">
         <v>-166</v>
       </c>
-      <c r="AH88" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI88" s="12" t="s">
         <v>87</v>
       </c>
@@ -11987,8 +12119,11 @@
       <c r="AP88" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ88" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
         <v>146</v>
       </c>
@@ -12068,27 +12203,25 @@
       <c r="AA89" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB89" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC89" s="12">
+      <c r="AB89" s="12"/>
+      <c r="AC89" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD89" s="12">
         <v>234</v>
       </c>
-      <c r="AD89" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AE89" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AF89" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG89" s="12">
+      <c r="AG89" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH89" s="12">
         <v>-24</v>
       </c>
-      <c r="AH89" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI89" s="12" t="s">
         <v>87</v>
       </c>
@@ -12113,8 +12246,11 @@
       <c r="AP89" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ89" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
         <v>147</v>
       </c>
@@ -12194,9 +12330,7 @@
       <c r="AA90" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB90" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB90" s="12"/>
       <c r="AC90" s="12" t="s">
         <v>87</v>
       </c>
@@ -12209,12 +12343,12 @@
       <c r="AF90" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG90" s="12">
+      <c r="AG90" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH90" s="12">
         <v>-24</v>
       </c>
-      <c r="AH90" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI90" s="12" t="s">
         <v>87</v>
       </c>
@@ -12239,8 +12373,11 @@
       <c r="AP90" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ90" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
         <v>137</v>
       </c>
@@ -12320,27 +12457,25 @@
       <c r="AA91" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB91" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC91" s="12">
+      <c r="AB91" s="12"/>
+      <c r="AC91" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD91" s="12">
         <v>18</v>
       </c>
-      <c r="AD91" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AE91" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AF91" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG91" s="12">
+      <c r="AG91" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH91" s="12">
         <v>-18</v>
       </c>
-      <c r="AH91" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI91" s="12" t="s">
         <v>87</v>
       </c>
@@ -12365,8 +12500,11 @@
       <c r="AP91" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ91" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
         <v>148</v>
       </c>
@@ -12446,27 +12584,25 @@
       <c r="AA92" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB92" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC92" s="12">
+      <c r="AB92" s="12"/>
+      <c r="AC92" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD92" s="12">
         <v>48</v>
       </c>
-      <c r="AD92" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AE92" s="12" t="s">
         <v>87</v>
       </c>
       <c r="AF92" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG92" s="12">
+      <c r="AG92" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH92" s="12">
         <v>48</v>
       </c>
-      <c r="AH92" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI92" s="12" t="s">
         <v>87</v>
       </c>
@@ -12491,8 +12627,11 @@
       <c r="AP92" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ92" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
         <v>149</v>
       </c>
@@ -12572,9 +12711,7 @@
       <c r="AA93" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AB93" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="AB93" s="12"/>
       <c r="AC93" s="12" t="s">
         <v>87</v>
       </c>
@@ -12587,12 +12724,12 @@
       <c r="AF93" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AG93" s="12">
+      <c r="AG93" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH93" s="12">
         <v>48</v>
       </c>
-      <c r="AH93" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="AI93" s="12" t="s">
         <v>87</v>
       </c>
@@ -12617,8 +12754,11 @@
       <c r="AP93" s="12" t="s">
         <v>87</v>
       </c>
+      <c r="AQ93" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
         <v>150</v>
       </c>
@@ -12698,53 +12838,54 @@
       <c r="AA94" s="12">
         <v>3577</v>
       </c>
-      <c r="AB94" s="12">
+      <c r="AB94" s="12"/>
+      <c r="AC94" s="12">
         <v>3795</v>
       </c>
-      <c r="AC94" s="12">
+      <c r="AD94" s="12">
         <v>4581</v>
       </c>
-      <c r="AD94" s="12">
+      <c r="AE94" s="12">
         <v>3634</v>
       </c>
-      <c r="AE94" s="12">
+      <c r="AF94" s="12">
         <v>4507</v>
       </c>
-      <c r="AF94" s="12">
+      <c r="AG94" s="12">
         <v>5230</v>
       </c>
-      <c r="AG94" s="12">
+      <c r="AH94" s="12">
         <v>6997</v>
       </c>
-      <c r="AH94" s="12">
+      <c r="AI94" s="12">
         <v>7291</v>
       </c>
-      <c r="AI94" s="12">
+      <c r="AJ94" s="12">
         <v>6335</v>
       </c>
-      <c r="AJ94" s="12">
+      <c r="AK94" s="12">
         <v>7040</v>
       </c>
-      <c r="AK94" s="12">
+      <c r="AL94" s="12">
         <v>4572</v>
       </c>
-      <c r="AL94" s="12">
+      <c r="AM94" s="12">
         <v>6334</v>
       </c>
-      <c r="AM94" s="12">
+      <c r="AN94" s="12">
         <v>5961</v>
       </c>
-      <c r="AN94" s="12">
+      <c r="AO94" s="12">
         <v>4343</v>
       </c>
-      <c r="AO94" s="12">
+      <c r="AP94" s="12">
         <v>4655</v>
       </c>
-      <c r="AP94" s="12">
+      <c r="AQ94" s="12">
         <v>7928</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>151</v>
       </c>
@@ -12789,6 +12930,7 @@
       <c r="AN95" s="7"/>
       <c r="AO95" s="7"/>
       <c r="AP95" s="7"/>
+      <c r="AQ95" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>